<commit_message>
notebook and files/compiled abi to make it work
</commit_message>
<xml_diff>
--- a/data/agents_data.xlsx
+++ b/data/agents_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescabianchessi/Documents/UNIVERSITA/DSBA_2/FINANCE/GROUP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cirib\repos\FinTech-\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E07367-4839-8245-A175-D07029D4368D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0DFA16-25C3-46DF-AAFC-3D86AA1E811F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2C24E830-EA44-584D-B2A2-118FF834EA71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C24E830-EA44-584D-B2A2-118FF834EA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,15 +41,9 @@
     <t>Bianchessi</t>
   </si>
   <si>
-    <t xml:space="preserve">Ilaria </t>
-  </si>
-  <si>
     <t>Bolla</t>
   </si>
   <si>
-    <t xml:space="preserve">Botti </t>
-  </si>
-  <si>
     <t>Davide</t>
   </si>
   <si>
@@ -60,9 +53,6 @@
     <t>Anna</t>
   </si>
   <si>
-    <t xml:space="preserve">Di Marco </t>
-  </si>
-  <si>
     <t>Comune</t>
   </si>
   <si>
@@ -72,9 +62,6 @@
     <t>Truck</t>
   </si>
   <si>
-    <t xml:space="preserve">Disposal Station </t>
-  </si>
-  <si>
     <t>Recycle</t>
   </si>
   <si>
@@ -129,10 +116,22 @@
     <t>recycle</t>
   </si>
   <si>
-    <t xml:space="preserve">Milano </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bologna </t>
+    <t>Ilaria</t>
+  </si>
+  <si>
+    <t>Di Marco</t>
+  </si>
+  <si>
+    <t>Disposal Station</t>
+  </si>
+  <si>
+    <t>Milano</t>
+  </si>
+  <si>
+    <t>Bologna</t>
+  </si>
+  <si>
+    <t>Botti</t>
   </si>
 </sst>
 </file>
@@ -491,52 +490,52 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -548,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -568,15 +567,15 @@
         <v>500</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -588,15 +587,15 @@
         <v>900</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -608,15 +607,15 @@
         <v>800</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -628,15 +627,15 @@
         <v>200</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -648,46 +647,46 @@
         <v>560</v>
       </c>
       <c r="I7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="I9" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1">
         <v>45.464199999999998</v>
@@ -696,18 +695,18 @@
         <v>9.19</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G11" s="1">
         <v>44.494900000000001</v>
@@ -716,7 +715,7 @@
         <v>11.342599999999999</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>